<commit_message>
db update - fixed missing id
</commit_message>
<xml_diff>
--- a/doc/MD databaza Carny.xlsx
+++ b/doc/MD databaza Carny.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="List1" sheetId="3" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">List1!$A$1:$M$198</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1495" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1496" uniqueCount="626">
   <si>
     <t>53500854</t>
   </si>
@@ -1899,6 +1902,9 @@
   </si>
   <si>
     <t>50° 0' 22.2752079" N, 14° 34' 26.2356377" E</t>
+  </si>
+  <si>
+    <t>53509750</t>
   </si>
 </sst>
 </file>
@@ -2032,7 +2038,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2048,9 +2054,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kancelář">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2088,7 +2094,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kancelář">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2160,7 +2166,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kancelář">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2312,8 +2318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="G206" sqref="G206"/>
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="E201" sqref="E201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="80.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5173,7 +5179,9 @@
         <v>607</v>
       </c>
       <c r="D92" s="5"/>
-      <c r="E92" s="6"/>
+      <c r="E92" s="6" t="s">
+        <v>625</v>
+      </c>
       <c r="F92" s="6" t="s">
         <v>266</v>
       </c>

</xml_diff>